<commit_message>
resonance tank of seconder is investigated
secondary resonance tank frequency is split from primary resonance. It causes current balancing
</commit_message>
<xml_diff>
--- a/WPT/LTspice/2p4s_makale modelleri/Test-Data/test datalar.xlsx
+++ b/WPT/LTspice/2p4s_makale modelleri/Test-Data/test datalar.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20359"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020E0A49-D1E1-4404-9EF1-468F442164D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="11" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Sayfa1" sheetId="6" r:id="rId10"/>
     <sheet name="Sayfa3" sheetId="5" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -139,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -361,9 +362,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="İyi" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nötr" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -640,11 +641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="A1:XFD1048576"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1571,7 +1572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView topLeftCell="H9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -3098,11 +3099,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:XFD1048576"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3672,11 +3673,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J22" sqref="A1:XFD1048576"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4246,11 +4247,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4820,7 +4821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5394,7 +5395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5968,7 +5969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6542,7 +6543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7116,10 +7117,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>

</xml_diff>